<commit_message>
fix the alignment calculation.
</commit_message>
<xml_diff>
--- a/Design_general_mem_alloc.xlsx
+++ b/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work_space\alpha_concurrent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9AB874-B953-4E5F-83E1-727218F22DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A30F8-E103-458F-8390-B292832E9917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2837,17 +2837,6 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>キャッシュラインサイズ </a:t>
-          </a:r>
-          <a:r>
             <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
@@ -2856,7 +2845,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>or std::</a:t>
+            <a:t>alignof(std::</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
@@ -2867,7 +2856,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>max_align_t</a:t>
+            <a:t>max_align_t)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
@@ -2878,7 +2867,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>の大きい方でアライメントされる。</a:t>
+            <a:t>でアライメントされる。</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -3002,103 +2991,6 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>17368</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>123264</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="吹き出し: 角を丸めた四角形 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C103547-7C8B-44EF-8214-21D2182EA1B5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="21231225" y="14159192"/>
-          <a:ext cx="2438960" cy="1988484"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRoundRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 5687"/>
-            <a:gd name="adj2" fmla="val -74635"/>
-            <a:gd name="adj3" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>キャッシュラインを分離してみた。が、メモリの無駄が多いし、パフォーマンス的にベターかどうかわからない。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="0" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>そもそも、キャッシュラインは、環境によって異なるし。。。</a:t>
-          </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -3560,8 +3452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="M4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U51" sqref="U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
refactor of member variable name
</commit_message>
<xml_diff>
--- a/Design_general_mem_alloc.xlsx
+++ b/Design_general_mem_alloc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work_space\alpha_concurrent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A30F8-E103-458F-8390-B292832E9917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA325C10-1138-41C8-9228-845BE539BB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,13 +211,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>親となる chunk_header_multi_slot へのポインタ</t>
-    <rPh sb="0" eb="1">
-      <t>オヤ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>pointer</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -264,6 +257,25 @@
     </rPh>
     <rPh sb="10" eb="12">
       <t>ホンタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>親となる chunk_header_multi_slot へのポインタ(解放処理の高速化の為)</t>
+    <rPh sb="0" eb="1">
+      <t>オヤ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>カイホウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="41" eb="44">
+      <t>コウソクカ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>タメ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1956,14 +1968,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>44822</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>190508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>3219449</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>661146</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>233370</xdr:rowOff>
     </xdr:to>
@@ -1980,8 +1992,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="25512712" y="6581783"/>
-          <a:ext cx="280987" cy="3214687"/>
+          <a:off x="24799597" y="5164939"/>
+          <a:ext cx="278186" cy="5905500"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -2177,13 +2189,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:colOff>2428876</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:colOff>672354</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2200,8 +2212,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15973425" y="3686175"/>
-          <a:ext cx="9515475" cy="4343400"/>
+          <a:off x="15943170" y="3658160"/>
+          <a:ext cx="8720978" cy="4301378"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3179,6 +3191,252 @@
             <a:t>copy</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>6722</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>62760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>3216088</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>105623</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="左中かっこ 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04A8B1F1-E6BE-4041-A3CE-7475BF72EBAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="25464106" y="5679288"/>
+          <a:ext cx="278186" cy="3209366"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 29610"/>
+            <a:gd name="adj2" fmla="val 54402"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1557618</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1456765</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="フリーフォーム: 図形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34FC386E-1A2A-4FF8-B8A4-6EDEBFF295AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9760324" y="2017059"/>
+          <a:ext cx="15688235" cy="5121088"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 15688235"/>
+            <a:gd name="connsiteY0" fmla="*/ 627529 h 5121088"/>
+            <a:gd name="connsiteX1" fmla="*/ 1288676 w 15688235"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 5121088"/>
+            <a:gd name="connsiteX2" fmla="*/ 11844617 w 15688235"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 5121088"/>
+            <a:gd name="connsiteX3" fmla="*/ 15688235 w 15688235"/>
+            <a:gd name="connsiteY3" fmla="*/ 5121088 h 5121088"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="15688235" h="5121088">
+              <a:moveTo>
+                <a:pt x="0" y="627529"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1288676" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="11844617" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="15688235" y="5121088"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>178734</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>89084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>246530</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>156881</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="吹き出し: 角を丸めた四角形 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D42FF4-2E04-4248-BEA4-3BE973C19091}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24170528" y="10230408"/>
+          <a:ext cx="3306296" cy="773767"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -61445"/>
+            <a:gd name="adj2" fmla="val -95813"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>nullptr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の場合、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>std::malloc</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>で確保された領域であることを示す。</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3452,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U51" sqref="U51"/>
+    <sheetView tabSelected="1" topLeftCell="P19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3667,60 +3925,60 @@
     </row>
     <row r="36" spans="24:28">
       <c r="X36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y36" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Y36" s="5" t="s">
+      <c r="Z36" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Z36" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="AA36" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AB36" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="24:28">
       <c r="X37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="24:28">
       <c r="X38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="24:28">
       <c r="X39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="24:28">
       <c r="X40" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>